<commit_message>
update README.md to include project images and enhance visual presentation
</commit_message>
<xml_diff>
--- a/dashboar xbox Student.xlsx
+++ b/dashboar xbox Student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b61142d5b1e3b342/projetos/DIO/Heineken/Desafio_Dashboard_in_Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="634" documentId="8_{C3982B17-7FC8-4C9F-A294-4DDC285FDED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{592183F6-0447-449E-957E-EE0FE2805CCE}"/>
+  <xr:revisionPtr revIDLastSave="636" documentId="8_{C3982B17-7FC8-4C9F-A294-4DDC285FDED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E84C45F3-F90D-4D83-9FC2-9FDE1BC980F6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="9" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
     <sheet name="A̳ssets" sheetId="1" state="hidden" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -1153,7 +1153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1188,7 +1188,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -2034,7 +2033,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[bases.xlsx]C̳álculos!tbl_dash</c:name>
+    <c:name>[dashboar xbox Student.xlsx]C̳álculos!tbl_dash</c:name>
     <c:fmtId val="7"/>
   </c:pivotSource>
   <c:chart>
@@ -2434,21 +2433,21 @@
           <a:gradFill flip="none" rotWithShape="1">
             <a:gsLst>
               <a:gs pos="0">
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:gs>
               <a:gs pos="75000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="51000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="100000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="20000"/>
                   <a:lumOff val="80000"/>
                   <a:alpha val="15000"/>
@@ -2537,7 +2536,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:dLblPos val="outEnd"/>
@@ -2561,21 +2560,21 @@
           <a:gradFill flip="none" rotWithShape="1">
             <a:gsLst>
               <a:gs pos="0">
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:gs>
               <a:gs pos="75000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="51000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="100000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="20000"/>
                   <a:lumOff val="80000"/>
                   <a:alpha val="15000"/>
@@ -2664,7 +2663,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
           <c:dLblPos val="outEnd"/>
@@ -2999,6 +2998,92 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2"/>
+                  </a:gs>
+                  <a:gs pos="75000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="51000">
+                    <a:schemeClr val="accent2">
+                      <a:alpha val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="20000"/>
+                      <a:lumOff val="80000"/>
+                      <a:alpha val="15000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-4003-4FD8-BB47-843FBE0983F6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2"/>
+                  </a:gs>
+                  <a:gs pos="75000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="51000">
+                    <a:schemeClr val="accent2">
+                      <a:alpha val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="20000"/>
+                      <a:lumOff val="80000"/>
+                      <a:alpha val="15000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-4003-4FD8-BB47-843FBE0983F6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -3074,7 +3159,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-BR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
               <c:dLblPos val="outEnd"/>
@@ -3168,7 +3253,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-BR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
               <c:dLblPos val="outEnd"/>
@@ -11921,7 +12006,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3287245-3A43-4671-9C2D-10C8A8F33D60}" name="Tabela dinâmica2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3287245-3A43-4671-9C2D-10C8A8F33D60}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B26:C29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -12610,7 +12695,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7CCF1A7-2335-4106-8E25-BAE1ACFF79EF}" name="Tabela dinâmica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7CCF1A7-2335-4106-8E25-BAE1ACFF79EF}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B16:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -13003,7 +13088,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2C6C2B8-61E0-491E-A11C-208A45E9DC15}" name="tbl_dash" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2C6C2B8-61E0-491E-A11C-208A45E9DC15}" name="tbl_dash" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="B8:D11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -26937,7 +27022,7 @@
       <c r="C9" s="17">
         <v>3847</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9">
         <v>147</v>
       </c>
       <c r="E9"/>
@@ -27241,7 +27326,7 @@
       <c r="C10" s="17">
         <v>3786</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10">
         <v>148</v>
       </c>
       <c r="E10"/>
@@ -27545,7 +27630,7 @@
       <c r="C11" s="17">
         <v>7633</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11">
         <v>295</v>
       </c>
       <c r="G11"/>
@@ -27678,7 +27763,7 @@
       <c r="B27" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27">
         <v>147</v>
       </c>
       <c r="D27"/>
@@ -27689,7 +27774,7 @@
       <c r="B28" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28">
         <v>148</v>
       </c>
       <c r="D28">
@@ -27703,7 +27788,7 @@
       <c r="B29" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29">
         <v>295</v>
       </c>
       <c r="E29"/>
@@ -36261,6 +36346,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010001E48B58A68BE64E9120D347E3E06B3A" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2f90046ec77328b7f86417d2e03b3d33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851b35d3-0456-4d6a-bc2f-da927e91d158" xmlns:ns3="19483571-f922-4e8e-9c1c-26f0a2252132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c815006ac2d4f05ee97fdd57e40d8e38" ns2:_="" ns3:_="">
     <xsd:import namespace="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
@@ -36515,27 +36620,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
+    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32608D25-EC36-42FE-A1DC-F778995A6799}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36552,23 +36656,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
-    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>